<commit_message>
Updated Test Data Deteleted NavigationBarPageObject
</commit_message>
<xml_diff>
--- a/Tests/SneakyPythonGitHubTestData.xlsx
+++ b/Tests/SneakyPythonGitHubTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mabdelmonem\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\SneakyPythonGitHub\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>UserName</t>
   </si>
@@ -35,9 +35,6 @@
     <t>IsValid</t>
   </si>
   <si>
-    <t>ahitsmo</t>
-  </si>
-  <si>
     <t>000000aa</t>
   </si>
   <si>
@@ -53,16 +50,25 @@
     <t>the Password has one upper case letter</t>
   </si>
   <si>
-    <t>Ahitsmo</t>
-  </si>
-  <si>
     <t>The UserName has one upper case letter</t>
   </si>
   <si>
-    <t>Ahitsm0</t>
-  </si>
-  <si>
     <t>The UserName has one incorrect letter</t>
+  </si>
+  <si>
+    <t>sneakypythontestuser</t>
+  </si>
+  <si>
+    <t>SneakyPythonTestUser</t>
+  </si>
+  <si>
+    <t>sn3akypythontestuser</t>
+  </si>
+  <si>
+    <t>The UserName is empty</t>
+  </si>
+  <si>
+    <t>The Password is empty</t>
   </si>
 </sst>
 </file>
@@ -380,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
@@ -405,63 +411,85 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Integartion Page Object and Tests
</commit_message>
<xml_diff>
--- a/Tests/SneakyPythonGitHubTestData.xlsx
+++ b/Tests/SneakyPythonGitHubTestData.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Projects\SneakyPythonGitHub\Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="FilterIntegration" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>UserName</t>
   </si>
@@ -69,6 +65,21 @@
   </si>
   <si>
     <t>The Password is empty</t>
+  </si>
+  <si>
+    <t>seacrh string</t>
+  </si>
+  <si>
+    <t>Atom</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>HUBoard</t>
+  </si>
+  <si>
+    <t>selenium</t>
   </si>
 </sst>
 </file>
@@ -166,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -388,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,4 +506,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>